<commit_message>
add exemplary clean_cells.json; correct values for testing will be extracted from such a json file
</commit_message>
<xml_diff>
--- a/test/test_cellparser.xlsx
+++ b/test/test_cellparser.xlsx
@@ -46,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="1">
+    <comment ref="G7" authorId="1">
       <text>
         <r>
           <rPr>
@@ -64,11 +64,11 @@
             <rFont val="Tahoma"/>
           </rPr>
           <t xml:space="preserve">
-CellParsingError</t>
+SeparatorCellError</t>
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="1">
+    <comment ref="H7" authorId="1">
       <text>
         <r>
           <rPr>
@@ -90,29 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t>walter.fuchs:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">
-SeparatorCellError</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J6" authorId="1">
+    <comment ref="I7" authorId="1">
       <text>
         <r>
           <rPr>
@@ -156,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="1">
+    <comment ref="G8" authorId="1">
       <text>
         <r>
           <rPr>
@@ -181,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="1">
+    <comment ref="H8" authorId="1">
       <text>
         <r>
           <rPr>
@@ -206,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0">
+    <comment ref="J8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -215,6 +193,28 @@
             <rFont val="Arial"/>
           </rPr>
           <t>Keep: [teʔiowaa]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>walter.fuchs:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+CellParsingError</t>
         </r>
       </text>
     </comment>
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>English</t>
   </si>
@@ -285,12 +285,6 @@
     <t>&lt;peteĩ&gt;(uno){Guasch1962:670}</t>
   </si>
   <si>
-    <t>one@</t>
-  </si>
-  <si>
-    <t>two</t>
-  </si>
-  <si>
     <t>dos</t>
   </si>
   <si>
@@ -379,6 +373,27 @@
   </si>
   <si>
     <t>French</t>
+  </si>
+  <si>
+    <t>&lt;peteĩ&gt;</t>
+  </si>
+  <si>
+    <t>&lt;irundy&gt;</t>
+  </si>
+  <si>
+    <t>three@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">four </t>
+  </si>
+  <si>
+    <t>cuatro</t>
+  </si>
+  <si>
+    <t>quatro</t>
+  </si>
+  <si>
+    <t>quatre</t>
   </si>
 </sst>
 </file>
@@ -433,7 +448,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,6 +507,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -569,12 +590,10 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -869,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -902,7 +921,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>4</v>
@@ -959,34 +978,36 @@
       <c r="G3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="13"/>
-      <c r="G4" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="15" t="s">
+      <c r="G4" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>48</v>
+      <c r="I4" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -994,99 +1015,123 @@
         <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>38</v>
+      <c r="G5" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>41</v>
+      <c r="G6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>47</v>
+        <v>38</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="22" t="s">
-        <v>33</v>
-      </c>
       <c r="J7" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="J8" s="24" t="s">
-        <v>43</v>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="J9" s="19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="J10" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="J11" s="19" t="s">
-        <v>50</v>
-      </c>
+      <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>